<commit_message>
added narratives to the findings
</commit_message>
<xml_diff>
--- a/data/RLIe_GET_L2.xlsx
+++ b/data/RLIe_GET_L2.xlsx
@@ -461,7 +461,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         <v>0.5894736842105264</v>
       </c>
       <c r="G14">
-        <v>0.7097744360902256</v>
+        <v>0.7067669172932332</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -878,10 +878,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F15">
-        <v>0.5684210526315789</v>
+        <v>0.5729323308270677</v>
       </c>
       <c r="G15">
-        <v>0.6947368421052631</v>
+        <v>0.6977443609022556</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         <v>0.5699248120300752</v>
       </c>
       <c r="G16">
-        <v>0.6947368421052631</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5699248120300752</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="G17">
-        <v>0.6962406015037594</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
         <v>0.8055555555555556</v>
       </c>
       <c r="G19">
-        <v>0.8855555555555555</v>
+        <v>0.8844444444444445</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7988611111111111</v>
+        <v>0.7999722222222223</v>
       </c>
       <c r="G20">
-        <v>0.8777777777777778</v>
+        <v>0.8766666666666667</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1088,7 +1088,7 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7944444444444445</v>
+        <v>0.7933333333333333</v>
       </c>
       <c r="G21">
         <v>0.8733333333333333</v>
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8934782608695653</v>
+        <v>0.8934239130434783</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1193,10 +1193,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F24">
-        <v>0.8695652173913043</v>
+        <v>0.8673913043478261</v>
       </c>
       <c r="G24">
-        <v>0.9652173913043478</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1228,10 +1228,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8717391304347826</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="G25">
-        <v>0.9652173913043478</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
narrative for fig 3 - Findings page
</commit_message>
<xml_diff>
--- a/data/RLIe_GET_L2.xlsx
+++ b/data/RLIe_GET_L2.xlsx
@@ -461,7 +461,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -843,10 +843,10 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5894736842105264</v>
+        <v>0.58796992481203</v>
       </c>
       <c r="G14">
-        <v>0.7067669172932332</v>
+        <v>0.7082706766917293</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -878,10 +878,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F15">
-        <v>0.5729323308270677</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G15">
-        <v>0.6977443609022556</v>
+        <v>0.6932706766917288</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -913,7 +913,7 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5699248120300752</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G16">
         <v>0.6962406015037594</v>
@@ -948,7 +948,7 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5684210526315789</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G17">
         <v>0.6947368421052631</v>
@@ -983,10 +983,10 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8333333333333334</v>
+        <v>0.8322222222222222</v>
       </c>
       <c r="G18">
-        <v>0.9044444444444444</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
         <v>0.8055555555555556</v>
       </c>
       <c r="G19">
-        <v>0.8844444444444445</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7999722222222223</v>
+        <v>0.7988888888888889</v>
       </c>
       <c r="G20">
-        <v>0.8766666666666667</v>
+        <v>0.8788888888888888</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         <v>0.7933333333333333</v>
       </c>
       <c r="G21">
-        <v>0.8733333333333333</v>
+        <v>0.8744444444444445</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8934239130434783</v>
+        <v>0.8913043478260869</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1161,7 +1161,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9630434782608696</v>
+        <v>0.9608695652173913</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F24">
-        <v>0.8673913043478261</v>
+        <v>0.8717391304347826</v>
       </c>
       <c r="G24">
         <v>0.9630434782608696</v>
@@ -1228,7 +1228,7 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8695652173913043</v>
+        <v>0.8695108695652174</v>
       </c>
       <c r="G25">
         <v>0.9630434782608696</v>

</xml_diff>

<commit_message>
Update Quarto workflow: install R for CI
</commit_message>
<xml_diff>
--- a/data/RLIe_GET_L2.xlsx
+++ b/data/RLIe_GET_L2.xlsx
@@ -496,7 +496,7 @@
         <v>0.34</v>
       </c>
       <c r="G4">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8363636363636364</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -846,7 +846,7 @@
         <v>0.58796992481203</v>
       </c>
       <c r="G14">
-        <v>0.7082706766917293</v>
+        <v>0.7097744360902256</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -881,7 +881,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="G15">
-        <v>0.6932706766917288</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="G16">
-        <v>0.6962406015037594</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5714285714285714</v>
+        <v>0.5669172932330827</v>
       </c>
       <c r="G17">
-        <v>0.6947368421052631</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -986,7 +986,7 @@
         <v>0.8322222222222222</v>
       </c>
       <c r="G18">
-        <v>0.9066666666666666</v>
+        <v>0.9055555555555556</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8055555555555556</v>
+        <v>0.8044444444444444</v>
       </c>
       <c r="G19">
         <v>0.8833333333333333</v>
@@ -1091,7 +1091,7 @@
         <v>0.7933333333333333</v>
       </c>
       <c r="G21">
-        <v>0.8744444444444445</v>
+        <v>0.8722499999999996</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8913043478260869</v>
+        <v>0.8934782608695653</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1161,7 +1161,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9608695652173913</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1193,10 +1193,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F24">
-        <v>0.8717391304347826</v>
+        <v>0.8716847826086956</v>
       </c>
       <c r="G24">
-        <v>0.9630434782608696</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8695108695652174</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="G25">
         <v>0.9630434782608696</v>

</xml_diff>